<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@fb8f41156457d44ac85662de3aa29290168164b6 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -8,13 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
-    <sheet name="Costs" sheetId="2" r:id="rId2"/>
-    <sheet name="Colors" sheetId="3" r:id="rId3"/>
+    <sheet name="DNF" sheetId="2" r:id="rId2"/>
+    <sheet name="Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="Costs (DNF)" sheetId="4" r:id="rId4"/>
+    <sheet name="Colors" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="1">'Costs'!$H$2</definedName>
+    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$H$2</definedName>
+    <definedName name="BoardQty" localSheetId="2">'Costs'!$H$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="1">'Costs'!$H$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
+    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$H$4</definedName>
+    <definedName name="TotalCost" localSheetId="2">'Costs'!$H$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -152,8 +157,140 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="G4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use the minimum extend price across distributors not taking account available quantities.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schematic identifier for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Description of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PCB footprint for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Manufacturer number for each part and link to it's datasheet (Ctrl-click).
+Purple -&gt; Obsolete part detected by one of the distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of each part needed.
+Gray -&gt; No manf# provided.
+Red -&gt; No parts available.
+Orange -&gt; Not enough parts available.
+Yellow -&gt; Parts available, but haven't purchased enough.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum unit price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum extended price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="115">
   <si>
     <t>Row</t>
   </si>
@@ -194,7 +331,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>C1 C2 C3 C4 C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98</t>
+    <t>C1 C2 C3 C4 C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C103 C104</t>
   </si>
   <si>
     <t>1uF</t>
@@ -203,55 +340,94 @@
     <t>C_0402_1005Metric</t>
   </si>
   <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Samsung%20PDFs/CL_Series_MLCC_ds.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL05A105KP5NNNC/3886734</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>C_Small</t>
+  </si>
+  <si>
+    <t>C101 C102 C105 C106</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>SK6812</t>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98</t>
+  </si>
+  <si>
+    <t>SK6812_EC15</t>
+  </si>
+  <si>
+    <t>LED_SK6812_EC15_1.5x1.5mm</t>
+  </si>
+  <si>
     <t>98</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/Samsung%20PDFs/CL_Series_MLCC_ds.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL05A105KP5NNNC/3886734</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>SK6812</t>
-  </si>
-  <si>
-    <t>D1 D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98</t>
-  </si>
-  <si>
-    <t>SK6812_EC15</t>
-  </si>
-  <si>
-    <t>LED_SK6812_EC15_1.5x1.5mm</t>
-  </si>
-  <si>
     <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/2384/CL05A105KP5NNN_Specsheet%20(1).pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/4492/11569136</t>
   </si>
   <si>
-    <t>3</t>
+    <t>OLED-128O064D</t>
+  </si>
+  <si>
+    <t>DS1 DS2</t>
+  </si>
+  <si>
+    <t>https://www.vishay.com/docs/37902/oled128o064dbpp3n00000.pdf</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>Conn_01x03_Pin</t>
   </si>
   <si>
-    <t>J1 J2</t>
+    <t>J1</t>
   </si>
   <si>
     <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Pin</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>OLED STEMMA</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
   <si>
     <t>R</t>
@@ -272,6 +448,39 @@
     <t>https://www.digikey.ch/en/products/detail/walsin-technology-corporation/WR04X3300FTL/13239224</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>R2 R4</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>R3 R5</t>
+  </si>
+  <si>
+    <t>390K</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>TLV810EA29DBZ</t>
+  </si>
+  <si>
+    <t>U1 U2</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/tlv803e.pdf</t>
+  </si>
+  <si>
     <t>KiBot Bill of Materials</t>
   </si>
   <si>
@@ -311,18 +520,30 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>199 (199 SMD/ 0 THT)</t>
+    <t>218 (205 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
+    <t>215 (204 SMD/ 0 THT)</t>
+  </si>
+  <si>
     <t>Number of PCBs:</t>
   </si>
   <si>
     <t>Total Components:</t>
   </si>
   <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>R6 R7</t>
+  </si>
+  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -338,18 +559,21 @@
     <t>Ext$</t>
   </si>
   <si>
-    <t>Unpolarized capacitor</t>
-  </si>
-  <si>
-    <t>RGB LED with integrated controller</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
+    <t>Unpolarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>OLED display 128x64</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x04, script generated</t>
   </si>
   <si>
     <t>Resistor</t>
   </si>
   <si>
+    <t>push-pull, active-high, 200mS reset delay, 2.93V threshold voltage, SOT-23</t>
+  </si>
+  <si>
     <t>Board Qty:</t>
   </si>
   <si>
@@ -362,7 +586,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-04 18:10:59</t>
+    <t>2024-10-05 14:05:18</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -528,7 +752,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,12 +804,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF0BD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF0FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -683,9 +901,6 @@
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -721,14 +936,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -813,8 +1028,112 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2378784</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>483309</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1140,7 +1459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1163,7 +1482,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1175,55 +1494,55 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F2" s="3">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1231,16 +1550,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="F6" s="3">
-        <v>199</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1307,7 +1626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="105" customHeight="1">
+    <row r="10" spans="1:10">
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
@@ -1323,84 +1642,276 @@
       <c r="E10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="105" customHeight="1">
+      <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1">
+      <c r="I11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="9" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="F12" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>38</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1415,7 +1926,218 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="51.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="32" customHeight="1">
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="C2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="C3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="C4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="C5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="C6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="8" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
@@ -1428,7 +2150,7 @@
   <cols>
     <col min="1" max="1" width="60.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="3" max="3" width="59.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="47.7109375" customWidth="1" outlineLevel="2"/>
     <col min="5" max="5" width="61.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1" outlineLevel="1"/>
@@ -1438,7 +2160,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1447,210 +2169,339 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="13">
+      <c r="G2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="15">
+      <c r="G3" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="14">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="16">
-        <f>SUM(H10:H13)</f>
+        <v>69</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="15">
+        <f>SUM(H10:H19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="A8" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>60</v>
+      <c r="E9" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" customHeight="1">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="C10" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="18">
+        <f>CEILING(BoardQty*102,1)</f>
+        <v>102</v>
+      </c>
+      <c r="H10" s="19">
+        <f>IF(AND(ISNUMBER(F10),ISNUMBER(G10)),F10*G10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="18">
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
+      </c>
+      <c r="H11" s="19">
+        <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="105" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="18">
         <f>CEILING(BoardQty*98,1)</f>
         <v>98</v>
       </c>
-      <c r="H10" s="20">
-        <f>IF(AND(ISNUMBER(F10),ISNUMBER(G10)),F10*G10,"")</f>
+      <c r="H12" s="19">
+        <f>IF(AND(ISNUMBER(F12),ISNUMBER(G12)),F12*G12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="105" customHeight="1">
-      <c r="A11" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="19">
-        <f>CEILING(BoardQty*98,1)</f>
-        <v>98</v>
-      </c>
-      <c r="H11" s="20">
-        <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="19">
+    <row r="13" spans="1:8">
+      <c r="A13" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="18">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="H12" s="20">
-        <f>IF(AND(ISNUMBER(F12),ISNUMBER(G12)),F12*G12,"")</f>
+      <c r="H13" s="19">
+        <f>IF(AND(ISNUMBER(F13),ISNUMBER(G13)),F13*G13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1">
-      <c r="A13" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="19">
+    <row r="14" spans="1:8">
+      <c r="A14" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="18">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="H13" s="20">
-        <f>IF(AND(ISNUMBER(F13),ISNUMBER(G13)),F13*G13,"")</f>
+      <c r="H14" s="19">
+        <f>IF(AND(ISNUMBER(F14),ISNUMBER(G14)),F14*G14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="23" t="s">
-        <v>70</v>
+    <row r="15" spans="1:8">
+      <c r="A15" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="18">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="19">
+        <f>IF(AND(ISNUMBER(F15),ISNUMBER(G15)),F15*G15,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" customHeight="1">
+      <c r="A16" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="18">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="19">
+        <f>IF(AND(ISNUMBER(F16),ISNUMBER(G16)),F16*G16,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="18">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="H17" s="19">
+        <f>IF(AND(ISNUMBER(F17),ISNUMBER(G17)),F17*G17,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="18">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="H18" s="19">
+        <f>IF(AND(ISNUMBER(F18),ISNUMBER(G18)),F18*G18,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="18">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="H19" s="19">
+        <f>IF(AND(ISNUMBER(F19),ISNUMBER(G19)),F19*G19,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="22" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1678,18 +2529,255 @@
       <formula>AND(ISBLANK(E13),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>AND(ISBLANK(E14),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>AND(ISBLANK(E15),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>AND(ISBLANK(E16),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>AND(ISBLANK(E17),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>AND(ISBLANK(E18),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="expression" dxfId="0" priority="10">
+      <formula>AND(ISBLANK(E19),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1"/>
-    <hyperlink ref="E11" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId2"/>
     <hyperlink ref="E13" r:id="rId3"/>
+    <hyperlink ref="E16" r:id="rId4"/>
+    <hyperlink ref="E19" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="8" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="32" customHeight="1">
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="D2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="D3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="14">
+        <f>TotalCost/BoardQty</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="D4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="15">
+        <f>SUM(H10:H11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="D5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="D6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="18">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="19">
+        <f>IF(AND(ISNUMBER(F10),ISNUMBER(G10)),F10*G10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="18">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="19">
+        <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="D1:H1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(ISBLANK(E10),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND(ISBLANK(E11),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -1702,77 +2790,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="24" t="s">
-        <v>77</v>
+      <c r="A8" s="23" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="25" t="s">
-        <v>78</v>
+      <c r="A9" s="24" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="26" t="s">
-        <v>79</v>
+      <c r="A10" s="25" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="27" t="s">
-        <v>80</v>
+      <c r="A11" s="26" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="28" t="s">
-        <v>81</v>
+      <c r="A12" s="27" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="29" t="s">
-        <v>82</v>
+      <c r="A13" s="28" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="30" t="s">
-        <v>83</v>
+      <c r="A14" s="29" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="31" t="s">
-        <v>84</v>
+      <c r="A15" s="30" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="32" t="s">
-        <v>85</v>
+      <c r="A16" s="31" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@69fa1f91c95806fd53bbb4cf03f6fd2894108b53 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -451,7 +451,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>R2 R4</t>
+    <t>R2</t>
   </si>
   <si>
     <t>10K</t>
@@ -472,7 +472,7 @@
     <t>TLV810EA29DBZ</t>
   </si>
   <si>
-    <t>U1 U2</t>
+    <t>U1</t>
   </si>
   <si>
     <t>SOT-23</t>
@@ -520,13 +520,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>218 (205 SMD/ 0 THT)</t>
+    <t>216 (205 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>215 (204 SMD/ 0 THT)</t>
+    <t>213 (204 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -586,7 +586,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-05 14:05:18</t>
+    <t>2024-10-05 16:27:13</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -1559,7 +1559,7 @@
         <v>80</v>
       </c>
       <c r="F6" s="3">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1838,7 +1838,7 @@
         <v>11</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>17</v>
@@ -1902,7 +1902,7 @@
         <v>61</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>17</v>
@@ -2026,7 +2026,7 @@
         <v>80</v>
       </c>
       <c r="F6" s="3">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2436,8 +2436,8 @@
         <v>11</v>
       </c>
       <c r="F17" s="18">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="H17" s="19">
         <f>IF(AND(ISNUMBER(F17),ISNUMBER(G17)),F17*G17,"")</f>
@@ -2483,8 +2483,8 @@
         <v>62</v>
       </c>
       <c r="F19" s="18">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="H19" s="19">
         <f>IF(AND(ISNUMBER(F19),ISNUMBER(G19)),F19*G19,"")</f>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@56bcfcf3832946813410f151d339cac758fd9e4f 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -8,13 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
-    <sheet name="Costs" sheetId="2" r:id="rId2"/>
-    <sheet name="Colors" sheetId="3" r:id="rId3"/>
+    <sheet name="DNF" sheetId="2" r:id="rId2"/>
+    <sheet name="Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="Costs (DNF)" sheetId="4" r:id="rId4"/>
+    <sheet name="Colors" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="1">'Costs'!$H$2</definedName>
+    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="2">'Costs'!$H$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="1">'Costs'!$H$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
+    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="2">'Costs'!$H$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -152,8 +157,127 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use the minimum extend price across distributors not taking account available quantities.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schematic identifier for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PCB footprint for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Manufacturer number for each part and link to it's datasheet (Ctrl-click).
+Purple -&gt; Obsolete part detected by one of the distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of each part needed.
+Gray -&gt; No manf# provided.
+Red -&gt; No parts available.
+Orange -&gt; Not enough parts available.
+Yellow -&gt; Parts available, but haven't purchased enough.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum unit price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum extended price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="96">
   <si>
     <t>Row</t>
   </si>
@@ -242,7 +366,10 @@
     <t>Conn_01x03_Pin</t>
   </si>
   <si>
-    <t>J1 J2</t>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>LED-IN</t>
   </si>
   <si>
     <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
@@ -341,12 +468,24 @@
     <t>Fitted Components:</t>
   </si>
   <si>
+    <t>201 (199 SMD/ 2 THT)</t>
+  </si>
+  <si>
     <t>Number of PCBs:</t>
   </si>
   <si>
     <t>Total Components:</t>
   </si>
   <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>LED-OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -377,7 +516,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-06 12:54:39</t>
+    <t>2024-10-06 13:13:09</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -828,8 +967,112 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2378784</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>950034</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1178,7 +1421,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1190,55 +1433,55 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F2" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1246,16 +1489,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F6" s="3">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1368,19 +1611,19 @@
         <v>29</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>11</v>
@@ -1388,22 +1631,22 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>10</v>
@@ -1412,7 +1655,7 @@
         <v>17</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>11</v>
@@ -1420,22 +1663,22 @@
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>10</v>
@@ -1444,30 +1687,30 @@
         <v>17</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>20</v>
@@ -1493,6 +1736,185 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="51.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="32" customHeight="1">
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="C5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -1506,7 +1928,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="60.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="55.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="47.7109375" customWidth="1" outlineLevel="2"/>
     <col min="5" max="5" width="61.7109375" customWidth="1" outlineLevel="1"/>
@@ -1517,7 +1939,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1526,13 +1948,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -1540,13 +1962,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -1555,13 +1977,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H15)</f>
@@ -1570,23 +1992,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -1610,16 +2032,16 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" customHeight="1">
@@ -1671,14 +2093,14 @@
         <v>29</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="H12" s="20">
         <f>IF(AND(ISNUMBER(F12),ISNUMBER(G12)),F12*G12,"")</f>
@@ -1687,16 +2109,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="19">
         <f>BoardQty*1</f>
@@ -1709,16 +2131,16 @@
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="19">
         <f>BoardQty*1</f>
@@ -1731,13 +2153,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -1750,15 +2172,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1807,7 +2229,179 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="32" customHeight="1">
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="15">
+        <f>TotalCost/BoardQty</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="16">
+        <f>SUM(G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="20">
+        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="D1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(ISBLANK(D10),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -1820,77 +2414,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@858d2dd1fb463c75b27bccf2da3ce8923a7aeb58 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -14,11 +14,11 @@
     <sheet name="Colors" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$H$2</definedName>
     <definedName name="BoardQty" localSheetId="2">'Costs'!$H$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$H$4</definedName>
     <definedName name="TotalCost" localSheetId="2">'Costs'!$H$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -163,7 +163,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0">
+    <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -211,11 +211,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Description of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>PCB footprint for each part.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -229,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="G9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="H9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -277,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="100">
   <si>
     <t>Row</t>
   </si>
@@ -462,7 +475,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>202 (200 SMD/ 2 THT)</t>
+    <t>204 (202 SMD/ 2 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -486,6 +499,15 @@
     <t xml:space="preserve"> (DNF)</t>
   </si>
   <si>
+    <t>R2 R3</t>
+  </si>
+  <si>
+    <t>3K3</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -516,10 +538,13 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-07 15:53:38</t>
+    <t>2024-10-08 08:38:54</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
+  </si>
+  <si>
+    <t>Resistor</t>
   </si>
   <si>
     <t>Columns colors</t>
@@ -1442,7 +1467,7 @@
         <v>59</v>
       </c>
       <c r="F2" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1737,7 +1762,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1781,7 +1806,7 @@
         <v>59</v>
       </c>
       <c r="F2" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1901,6 +1926,38 @@
         <v>32</v>
       </c>
       <c r="J9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="10" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1954,7 +2011,7 @@
         <v>50</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -1968,7 +2025,7 @@
         <v>52</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -1983,7 +2040,7 @@
         <v>54</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H15)</f>
@@ -2008,7 +2065,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2032,16 +2089,16 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" customHeight="1">
@@ -2115,7 +2172,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>37</v>
@@ -2172,15 +2229,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2231,11 +2288,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <pane xSplit="8" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -2244,66 +2301,68 @@
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1" outlineLevel="2"/>
     <col min="5" max="5" width="19.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" customHeight="1">
+    <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="13">
+      <c r="G2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="15">
+      <c r="G3" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="16">
-        <f>SUM(G10)</f>
+      <c r="G4" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="16">
+        <f>SUM(H10:H11)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
         <v>55</v>
       </c>
@@ -2311,7 +2370,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
         <v>57</v>
       </c>
@@ -2319,9 +2378,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2329,8 +2388,9 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
@@ -2338,61 +2398,91 @@
         <v>4</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>70</v>
-      </c>
       <c r="E9" s="18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>75</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="D10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="19">
+      <c r="F10" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G10" s="20">
-        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+      <c r="H10" s="20">
+        <f>IF(AND(ISNUMBER(F10),ISNUMBER(G10)),F10*G10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="23" t="s">
-        <v>80</v>
+    <row r="11" spans="1:8">
+      <c r="A11" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="19">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="20">
+        <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="23" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="D1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="F10">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(ISBLANK(D10),TRUE())</formula>
+      <formula>AND(ISBLANK(E10),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND(ISBLANK(E11),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2414,77 +2504,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@88b9b02c9c6b1ac4ea716c600346aba88077f420 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -454,13 +454,13 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>0.0.0-RC1</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2024-10-05</t>
+    <t>2024-10-16</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -538,7 +538,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-15 14:12:12</t>
+    <t>2024-10-16 16:47:02</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@45c584ff948b376296df0969ae1c252126cca136 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -454,7 +454,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1-RC</t>
   </si>
   <si>
     <t>Date:</t>
@@ -538,7 +538,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-16 16:57:15</t>
+    <t>2024-10-16 20:06:21</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@84a78cd54d30ba06f3ff6b812d09c0aadd561d98 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="105">
   <si>
     <t>Row</t>
   </si>
@@ -382,7 +382,7 @@
     <t>J1</t>
   </si>
   <si>
-    <t>LED-IN</t>
+    <t>JST PH 3</t>
   </si>
   <si>
     <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
@@ -400,42 +400,54 @@
     <t>J3</t>
   </si>
   <si>
+    <t>JST PH 4</t>
+  </si>
+  <si>
+    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>R_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>https://www.passivecomponent.com/wp-content/uploads/chipR/ASC_WR.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/walsin-technology-corporation/WR04X3300FTL/13239224</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>OLED</t>
   </si>
   <si>
-    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>R_0402_1005Metric</t>
-  </si>
-  <si>
-    <t>https://www.passivecomponent.com/wp-content/uploads/chipR/ASC_WR.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/en/products/detail/walsin-technology-corporation/WR04X3300FTL/13239224</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>U1 U2</t>
   </si>
   <si>
+    <t>OLED I2C</t>
+  </si>
+  <si>
     <t>OLED_128x128</t>
   </si>
   <si>
+    <t>img/GME12812.pdf</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005005253671396.html</t>
+  </si>
+  <si>
     <t>KiBot Bill of Materials</t>
   </si>
   <si>
@@ -493,9 +505,6 @@
     <t>J2</t>
   </si>
   <si>
-    <t>LED-OUT</t>
-  </si>
-  <si>
     <t xml:space="preserve"> (DNF)</t>
   </si>
   <si>
@@ -508,6 +517,12 @@
     <t>R_0805_2012Metric</t>
   </si>
   <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/stackpole-electronics-inc/RMCF0805FT3K30/1760325</t>
+  </si>
+  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -538,7 +553,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-16 20:06:21</t>
+    <t>2024-10-17 12:10:09</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -1097,7 +1112,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>950034</xdr:colOff>
+      <xdr:colOff>883359</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1446,7 +1461,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1458,13 +1473,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3">
         <v>8</v>
@@ -1472,41 +1487,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1514,13 +1529,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F6" s="3">
         <v>201</v>
@@ -1726,16 +1741,16 @@
         <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>20</v>
@@ -1743,11 +1758,11 @@
       <c r="H14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>11</v>
+      <c r="I14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1779,13 +1794,13 @@
     <col min="6" max="6" width="51.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="55.7109375" customWidth="1"/>
+    <col min="10" max="10" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1797,13 +1812,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3">
         <v>8</v>
@@ -1811,41 +1826,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1853,13 +1868,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F6" s="3">
         <v>201</v>
@@ -1908,10 +1923,10 @@
         <v>28</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>31</v>
@@ -1920,7 +1935,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>32</v>
@@ -1929,7 +1944,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="30" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
@@ -1940,25 +1955,25 @@
         <v>39</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>11</v>
+        <v>71</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1996,7 +2011,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2005,13 +2020,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -2019,13 +2034,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2034,13 +2049,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H15)</f>
@@ -2049,23 +2064,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2089,16 +2104,16 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" customHeight="1">
@@ -2172,7 +2187,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>37</v>
@@ -2210,13 +2225,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2229,15 +2244,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2300,10 +2315,10 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="47.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
@@ -2311,7 +2326,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2320,13 +2335,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -2334,13 +2349,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2349,13 +2364,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H11)</f>
@@ -2364,23 +2379,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2404,24 +2419,24 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="19" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>31</v>
@@ -2437,16 +2452,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="19" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="F11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2459,15 +2477,15 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="21" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="23" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2485,9 +2503,12 @@
       <formula>AND(ISBLANK(E11),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2504,77 +2525,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@ed3734ce3d0df49cb64748a579eb3f9c6220c56b 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -367,10 +367,10 @@
     <t>LED_SK6812_EC15_1.5x1.5mm</t>
   </si>
   <si>
-    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/2384/CL05A105KP5NNN_Specsheet%20(1).pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/4492/11569136</t>
+    <t>https://www.inolux-corp.com/datasheet/SMDLED/Addressable%20LED/IN-PI15TAT5R5G5B_v1.0.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/inolux/IN-PI15TAT5R5G5B/14555725</t>
   </si>
   <si>
     <t>3</t>
@@ -553,7 +553,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-17 12:10:09</t>
+    <t>2024-10-17 12:19:50</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@c1891d69b255ff34682b8087a0282670555ebd9c 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="107">
   <si>
     <t>Row</t>
   </si>
@@ -388,7 +388,10 @@
     <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
   </si>
   <si>
-    <t>~</t>
+    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc/B3B-PH-SM4-TB/926832</t>
   </si>
   <si>
     <t>4</t>
@@ -406,6 +409,9 @@
     <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
@@ -553,7 +559,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-17 12:19:50</t>
+    <t>2024-10-17 12:27:49</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -1461,7 +1467,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1473,13 +1479,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F2" s="3">
         <v>8</v>
@@ -1487,41 +1493,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1529,13 +1535,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F6" s="3">
         <v>201</v>
@@ -1637,7 +1643,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1662,31 +1668,31 @@
       <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="J11" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>10</v>
@@ -1694,31 +1700,31 @@
       <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>11</v>
+      <c r="J12" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>10</v>
@@ -1727,30 +1733,30 @@
         <v>17</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>20</v>
@@ -1759,10 +1765,10 @@
         <v>17</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1800,7 +1806,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1812,13 +1818,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F2" s="3">
         <v>8</v>
@@ -1826,41 +1832,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1868,13 +1874,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F6" s="3">
         <v>201</v>
@@ -1912,7 +1918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1923,7 +1929,7 @@
         <v>28</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>30</v>
@@ -1935,13 +1941,13 @@
         <v>10</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>11</v>
+      <c r="J9" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1">
@@ -1952,28 +1958,28 @@
         <v>11</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2011,7 +2017,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2020,13 +2026,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -2034,13 +2040,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2049,13 +2055,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H15)</f>
@@ -2064,23 +2070,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2104,16 +2110,16 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" customHeight="1">
@@ -2170,6 +2176,9 @@
       <c r="D12" s="19" t="s">
         <v>31</v>
       </c>
+      <c r="E12" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="F12" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
@@ -2181,16 +2190,19 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="F13" s="19">
         <f>BoardQty*1</f>
@@ -2203,16 +2215,16 @@
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F14" s="19">
         <f>BoardQty*1</f>
@@ -2225,13 +2237,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2244,15 +2256,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2293,11 +2305,13 @@
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1"/>
     <hyperlink ref="E11" r:id="rId2"/>
-    <hyperlink ref="E14" r:id="rId3"/>
+    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="E13" r:id="rId4"/>
+    <hyperlink ref="E14" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -2326,7 +2340,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2335,13 +2349,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -2349,13 +2363,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2364,13 +2378,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H11)</f>
@@ -2379,23 +2393,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2419,27 +2433,30 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>31</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="F10" s="19">
         <f>BoardQty*1</f>
@@ -2452,19 +2469,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2477,15 +2494,15 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2504,11 +2521,12 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1"/>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E11" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2525,77 +2543,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@c057869bc666828a260b41d334b71f5a277ae765 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-display-bom.xlsx
@@ -484,7 +484,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>8.0.4+1</t>
+    <t>8.0.6+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -559,10 +559,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-17 12:27:49</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
+    <t>2024-12-15 21:06:10</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.19 + KiBot v1.8.2</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -961,10 +961,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>16584</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>357600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>297815</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -991,7 +991,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1013,10 +1013,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>16584</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3024600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1043,7 +1043,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1065,10 +1065,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2378784</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>786225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1095,7 +1095,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1117,10 +1117,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>883359</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>290925</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1147,7 +1147,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>